<commit_message>
1. Refactor into energy_model and test --- 2. Start development on Sensor and Meter classes
</commit_message>
<xml_diff>
--- a/twin4build/test/data/configuration_template_1space_1v_1h_0c.xlsx
+++ b/twin4build/test/data/configuration_template_1space_1v_1h_0c.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://syddanskuni-my.sharepoint.com/personal/jabj_mmmi_sdu_dk/Documents/PhD_Project_Jakob/Twin4build/python/BuildingEnergyModel/BuildingEnergyModel/twin4build/test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="143" documentId="6_{BFA7A2FF-EE31-474C-9095-512E26FEE44B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B87E0F01-575D-41B0-80E3-4D6B0563D5E7}"/>
+  <xr:revisionPtr revIDLastSave="147" documentId="6_{BFA7A2FF-EE31-474C-9095-512E26FEE44B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A78C5933-369B-490A-8704-524F3171A0DE}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-105" windowWidth="38640" windowHeight="21240" xr2:uid="{0A98B5A4-E8E7-4876-BAF5-D3C6F6E2C062}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{0A98B5A4-E8E7-4876-BAF5-D3C6F6E2C062}"/>
   </bookViews>
   <sheets>
     <sheet name="Systems" sheetId="3" r:id="rId1"/>
@@ -724,7 +724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B0F6D5-8A47-48C4-A8B6-AFC37A61DB0A}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -800,7 +800,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E88391AB-9A45-440E-B7CA-6D31485712DF}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -845,7 +847,7 @@
   <dimension ref="A1:X1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5997,8 +5999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9F9D35B-B713-4EC3-BA55-A4EE8F2F331C}">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6082,7 +6084,7 @@
         <v>25</v>
       </c>
       <c r="N2">
-        <f>5*50*500</f>
+        <f>125000</f>
         <v>125000</v>
       </c>
     </row>
@@ -12042,7 +12044,7 @@
   <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21435,7 +21437,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{5F303923-A133-43EE-BF6A-9A627B0041CB}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21447,7 +21449,7 @@
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27467,7 +27469,7 @@
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33520,7 +33522,7 @@
   <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39584,7 +39586,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Remove dependency on building_data_collection_dict.py and add scaling values to kwargs in LSTM class
</commit_message>
<xml_diff>
--- a/twin4build/test/data/configuration_template_1space_1v_1h_0c.xlsx
+++ b/twin4build/test/data/configuration_template_1space_1v_1h_0c.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -5999,7 +5999,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9F9D35B-B713-4EC3-BA55-A4EE8F2F331C}">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>

</xml_diff>